<commit_message>
D8MT-1100: Update the mapping templates (EWCMS 1.17.0).
</commit_message>
<xml_diff>
--- a/templates/assets_mapping_template.xlsx
+++ b/templates/assets_mapping_template.xlsx
@@ -5,22 +5,24 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="D7 Inventory" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="MAPPING - ... to AV Portal Photo (av_portal_photo)" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="MAPPING - ... to AV Portal Video (av_portal_video)" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="MAPPING - ... to Document (document)" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="MAPPING - ... to Image (image)" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="MAPPING - ... to Remote video (remote_video)" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="MAPPING - ... to Video iframe (video_iframe)" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="MAPPING - ... to Webtools chart (webtools_chart)" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="MAPPING - ... to Webtools map (webtools_map)" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="MAPPING - ... to Webtools social feed (webtools_social_feed)" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="MAPPING - ... to iframe (iframe)" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="MAPPING - ... to Image (image)" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="MAPPING - ... to Remote video (remote_video)" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="MAPPING - ... to Video iframe (video_iframe)" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="MAPPING - ... to Webtools chart (webtools_chart)" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="MAPPING - ... to Webtools map (webtools_map)" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="MAPPING - ... to Webtools op publication list (webtools_op_publication_list)" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="MAPPING - ... to Webtools social feed (webtools_social_feed)" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="tbl_dest" vbProcedure="false">'MAPPING - ... to AV Portal Photo (av_portal_photo)'!$C$2:$I$37</definedName>
+    <definedName function="false" hidden="false" name="tbl_dest" vbProcedure="false">'MAPPING - ... to AV Portal Photo (av_portal_photo)'!$C$2:$I$10</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="106">
   <si>
     <t xml:space="preserve">Label</t>
   </si>
@@ -79,114 +81,111 @@
     <t xml:space="preserve">Field cardinality</t>
   </si>
   <si>
-    <t xml:space="preserve">bundle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Media type</t>
+    <t xml:space="preserve">uid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authored by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varchar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thumbnail/target_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thumbnail / target_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thumbnail/alt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thumbnail / alt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thumbnail/title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thumbnail / title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authored on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_media_avportal_photo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Media AV Portal Photo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AV Portal Video (av_portal_video)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_media_avportal_video</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Media AV Portal Video</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document (document)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ewcms_description/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description / value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ewcms_file_thumbnail/target_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ewcms_file_thumbnail/alt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ewcms_file_thumbnail/title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ewcms_publication_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publication date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ewcms_resource_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource type</t>
   </si>
   <si>
     <t xml:space="preserve">varchar_ascii</t>
   </si>
   <si>
-    <t xml:space="preserve">FALSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Authored by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">varchar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">thumbnail/alt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thumbnail / alt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">thumbnail/title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thumbnail / title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">created</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Authored on</t>
-  </si>
-  <si>
-    <t xml:space="preserve">changed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Changed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">default_langcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default translation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oe_media_avportal_photo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Media AV Portal Photo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AV Portal Video (av_portal_video)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Published</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oe_media_avportal_video</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Media AV Portal Video</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document (document)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ewcms_description/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description / value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ewcms_publication_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Publication date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ewcms_resource_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource type</t>
-  </si>
-  <si>
     <t xml:space="preserve">ewcms_subject</t>
   </si>
   <si>
@@ -208,6 +207,24 @@
     <t xml:space="preserve">Vocabularies / target_id</t>
   </si>
   <si>
+    <t xml:space="preserve">oe_media_file/target_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File / target_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_media_file/display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File / display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_media_file/description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File / description</t>
+  </si>
+  <si>
     <t xml:space="preserve">oe_media_file_type</t>
   </si>
   <si>
@@ -226,21 +243,78 @@
     <t xml:space="preserve">Remote File / title</t>
   </si>
   <si>
+    <t xml:space="preserve">oe_media_remote_file/size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remote File / size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iframe (iframe)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ewcms_media_caption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_media_iframe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iframe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_media_iframe_ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_media_iframe_thumbnail/target_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iframe thumbnail / target_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_media_iframe_thumbnail/alt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iframe thumbnail / alt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_media_iframe_thumbnail/title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iframe thumbnail / title</t>
+  </si>
+  <si>
     <t xml:space="preserve">Image (image)</t>
   </si>
   <si>
-    <t xml:space="preserve">ewcms_media_caption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caption</t>
-  </si>
-  <si>
     <t xml:space="preserve">ewcms_media_copyright</t>
   </si>
   <si>
     <t xml:space="preserve">Copyright</t>
   </si>
   <si>
+    <t xml:space="preserve">oe_media_image/target_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image / target_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_media_image/alt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image / alt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_media_image/title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image / title</t>
+  </si>
+  <si>
     <t xml:space="preserve">Remote video (remote_video)</t>
   </si>
   <si>
@@ -253,18 +327,6 @@
     <t xml:space="preserve">Video iframe (video_iframe)</t>
   </si>
   <si>
-    <t xml:space="preserve">oe_media_iframe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iframe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oe_media_iframe_ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ratio</t>
-  </si>
-  <si>
     <t xml:space="preserve">Webtools chart (webtools_chart)</t>
   </si>
   <si>
@@ -278,6 +340,12 @@
   </si>
   <si>
     <t xml:space="preserve">Webtools map snippet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Webtools op publication list (webtools_op_publication_list)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Webtools OP Publication lists snippet</t>
   </si>
   <si>
     <t xml:space="preserve">Webtools social feed (webtools_social_feed)</t>
@@ -374,7 +442,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -409,10 +477,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -495,18 +559,18 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K33" activeCellId="0" sqref="K33"/>
+      <selection pane="topLeft" activeCell="J42" activeCellId="0" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="6.75"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="7.83163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -547,27 +611,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y11"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
+      <selection pane="bottomLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="38.2040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.25"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.6377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -575,7 +639,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -585,8 +649,8 @@
       <c r="I1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="n">
-        <v>2438</v>
+      <c r="A2" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>7</v>
@@ -632,42 +696,42 @@
       <c r="D3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="0" t="n">
+      <c r="E3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="0" t="n">
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -678,157 +742,690 @@
       <c r="D5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="0" t="n">
+      <c r="E5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="0" t="n">
+      <c r="E6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="0" t="n">
+      <c r="E7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="0" t="n">
+      <c r="E8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="0" t="n">
+      <c r="E9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Y10"/>
+  <sheetViews>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="52.9795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="9" t="s">
+      <c r="D4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Y10"/>
+  <sheetViews>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="39.7755102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="0" t="n">
+      <c r="D4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -848,27 +1445,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y11"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="bottomLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.1632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.0510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -940,7 +1537,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="7" t="n">
         <v>0</v>
@@ -951,19 +1548,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H4" s="7" t="n">
         <v>0</v>
@@ -980,13 +1577,13 @@
         <v>24</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="7" t="n">
         <v>0</v>
@@ -997,16 +1594,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>27</v>
-      </c>
       <c r="E6" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>18</v>
@@ -1020,16 +1617,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>18</v>
@@ -1043,13 +1640,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="E8" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>18</v>
@@ -1066,13 +1663,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="E9" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>18</v>
@@ -1089,47 +1686,24 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="E10" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H10" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I10" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1149,27 +1723,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y12"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1177,7 +1751,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -1234,226 +1808,180 @@
       <c r="D3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="0" t="n">
+      <c r="E3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1473,27 +2001,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y19"/>
+  <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="bottomLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.3061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.8877551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1501,7 +2029,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -1565,7 +2093,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="7" t="n">
         <v>0</v>
@@ -1576,19 +2104,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H4" s="7" t="n">
         <v>0</v>
@@ -1605,13 +2133,13 @@
         <v>24</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="7" t="n">
         <v>0</v>
@@ -1622,13 +2150,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>27</v>
-      </c>
       <c r="E6" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>18</v>
@@ -1645,13 +2173,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>18</v>
@@ -1668,13 +2196,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="E8" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>18</v>
@@ -1691,13 +2219,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="E9" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>18</v>
@@ -1714,16 +2242,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>18</v>
@@ -1737,16 +2265,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>18</v>
@@ -1760,13 +2288,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>18</v>
@@ -1783,19 +2311,19 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>18</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H13" s="7" t="n">
         <v>0</v>
@@ -1806,13 +2334,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>18</v>
@@ -1823,42 +2351,42 @@
       <c r="H14" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I14" s="7" t="s">
-        <v>53</v>
+      <c r="I14" s="7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>18</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H15" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I15" s="7" t="s">
-        <v>53</v>
+      <c r="I15" s="7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>18</v>
@@ -1870,44 +2398,44 @@
         <v>0</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H17" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I17" s="7" t="n">
-        <v>1</v>
+      <c r="I17" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>18</v>
@@ -1915,30 +2443,168 @@
       <c r="H18" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I18" s="7" t="n">
-        <v>1</v>
+      <c r="I18" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="E21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="7" t="n">
+      <c r="D22" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1958,27 +2624,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y12"/>
+  <dimension ref="A1:Y15"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.3520408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.9387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1986,7 +2652,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -2050,7 +2716,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="7" t="n">
         <v>0</v>
@@ -2061,19 +2727,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H4" s="7" t="n">
         <v>0</v>
@@ -2090,13 +2756,13 @@
         <v>24</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="7" t="n">
         <v>0</v>
@@ -2107,16 +2773,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>27</v>
-      </c>
       <c r="E6" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>18</v>
@@ -2130,16 +2796,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>18</v>
@@ -2153,13 +2819,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="E8" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>18</v>
@@ -2176,13 +2842,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="E9" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>18</v>
@@ -2199,16 +2865,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>18</v>
@@ -2222,19 +2888,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H11" s="7" t="n">
         <v>0</v>
@@ -2245,16 +2911,16 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>18</v>
@@ -2263,6 +2929,75 @@
         <v>0</v>
       </c>
       <c r="I12" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2282,27 +3017,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y11"/>
+  <dimension ref="A1:Y14"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.7857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.0765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.9642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2310,7 +3045,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -2374,7 +3109,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="7" t="n">
         <v>0</v>
@@ -2385,19 +3120,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H4" s="7" t="n">
         <v>0</v>
@@ -2414,13 +3149,13 @@
         <v>24</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="7" t="n">
         <v>0</v>
@@ -2431,16 +3166,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>27</v>
-      </c>
       <c r="E6" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>18</v>
@@ -2454,16 +3189,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>18</v>
@@ -2477,13 +3212,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="E8" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>18</v>
@@ -2500,13 +3235,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="E9" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>18</v>
@@ -2523,16 +3258,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>18</v>
@@ -2546,24 +3281,93 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H11" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I11" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2583,27 +3387,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y15"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.1275510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.8571428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8010204081633"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2611,7 +3415,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -2675,10 +3479,10 @@
         <v>18</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I3" s="7" t="n">
         <v>1</v>
@@ -2686,22 +3490,22 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H4" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I4" s="7" t="n">
         <v>1</v>
@@ -2715,16 +3519,16 @@
         <v>24</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I5" s="7" t="n">
         <v>1</v>
@@ -2732,22 +3536,22 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>27</v>
-      </c>
       <c r="E6" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>18</v>
       </c>
       <c r="H6" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I6" s="7" t="n">
         <v>1</v>
@@ -2755,16 +3559,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>18</v>
@@ -2778,13 +3582,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="E8" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>18</v>
@@ -2793,7 +3597,7 @@
         <v>18</v>
       </c>
       <c r="H8" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I8" s="7" t="n">
         <v>1</v>
@@ -2801,13 +3605,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="E9" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>18</v>
@@ -2816,7 +3620,7 @@
         <v>18</v>
       </c>
       <c r="H9" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I9" s="7" t="n">
         <v>1</v>
@@ -2824,139 +3628,24 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H10" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I10" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="I14" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="I15" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2976,27 +3665,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y11"/>
+  <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.9387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3004,7 +3693,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -3068,10 +3757,10 @@
         <v>18</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I3" s="7" t="n">
         <v>1</v>
@@ -3079,22 +3768,22 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H4" s="7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I4" s="7" t="n">
         <v>1</v>
@@ -3108,16 +3797,16 @@
         <v>24</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I5" s="7" t="n">
         <v>1</v>
@@ -3125,13 +3814,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>27</v>
-      </c>
       <c r="E6" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>18</v>
@@ -3140,7 +3829,7 @@
         <v>18</v>
       </c>
       <c r="H6" s="7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I6" s="7" t="n">
         <v>1</v>
@@ -3148,13 +3837,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>18</v>
@@ -3171,13 +3860,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="E8" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>18</v>
@@ -3186,7 +3875,7 @@
         <v>18</v>
       </c>
       <c r="H8" s="7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I8" s="7" t="n">
         <v>1</v>
@@ -3194,13 +3883,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="E9" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>18</v>
@@ -3209,7 +3898,7 @@
         <v>18</v>
       </c>
       <c r="H9" s="7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I9" s="7" t="n">
         <v>1</v>
@@ -3217,16 +3906,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>18</v>
@@ -3240,24 +3929,162 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D15" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="7" t="n">
+      <c r="E15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3277,27 +4104,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y11"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.3571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.1836734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3305,7 +4132,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -3369,7 +4196,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="7" t="n">
         <v>0</v>
@@ -3380,19 +4207,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H4" s="7" t="n">
         <v>0</v>
@@ -3409,13 +4236,13 @@
         <v>24</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="7" t="n">
         <v>0</v>
@@ -3426,13 +4253,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>27</v>
-      </c>
       <c r="E6" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>18</v>
@@ -3449,13 +4276,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>18</v>
@@ -3472,13 +4299,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="E8" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>18</v>
@@ -3495,13 +4322,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="E9" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>18</v>
@@ -3518,47 +4345,24 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H10" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I10" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="7" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
D8MT-1100: Update the mapping templates (EWCMS 1.18.0).
</commit_message>
<xml_diff>
--- a/templates/assets_mapping_template.xlsx
+++ b/templates/assets_mapping_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="D7 Inventory" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
     <sheet name="MAPPING - ... to Webtools social feed (webtools_social_feed)" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="tbl_dest" vbProcedure="false">'MAPPING - ... to AV Portal Photo (av_portal_photo)'!$C$2:$I$10</definedName>
+    <definedName function="false" hidden="false" name="tbl_dest" vbProcedure="false">'MAPPING - ... to AV Portal Photo (av_portal_photo)'!$C$2:$I$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="112">
   <si>
     <t xml:space="preserve">Label</t>
   </si>
@@ -288,6 +288,18 @@
     <t xml:space="preserve">Iframe thumbnail / title</t>
   </si>
   <si>
+    <t xml:space="preserve">oe_media_iframe_thumbnail/width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iframe thumbnail / width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_media_iframe_thumbnail/height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iframe thumbnail / height</t>
+  </si>
+  <si>
     <t xml:space="preserve">Image (image)</t>
   </si>
   <si>
@@ -325,6 +337,12 @@
   </si>
   <si>
     <t xml:space="preserve">Video iframe (video_iframe)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ewcms_description/format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description / format</t>
   </si>
   <si>
     <t xml:space="preserve">Webtools chart (webtools_chart)</t>
@@ -558,19 +576,19 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J42" activeCellId="0" sqref="J42"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -616,22 +634,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+      <selection pane="bottomLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.25"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.6377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.61224489795918"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -639,7 +657,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -852,10 +870,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>41</v>
@@ -894,22 +912,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="52.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="52.3775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.61224489795918"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -917,7 +935,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -1130,10 +1148,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>41</v>
@@ -1169,25 +1187,25 @@
   </sheetPr>
   <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+      <selection pane="bottomLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="39.7755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="39.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.61224489795918"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1195,7 +1213,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -1408,10 +1426,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>41</v>
@@ -1450,22 +1468,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+      <selection pane="bottomLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.1632653061224"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.0510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.61224489795918"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1580,7 +1598,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>18</v>
@@ -1728,22 +1746,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.6071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.61224489795918"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2006,22 +2024,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="bottomLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.8877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.61224489795918"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2624,27 +2642,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y15"/>
+  <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.3520408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.9387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.6224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.61224489795918"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2998,6 +3016,52 @@
         <v>0</v>
       </c>
       <c r="I15" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3022,22 +3086,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+      <selection pane="bottomLeft" activeCell="K34" activeCellId="0" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.9642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.61224489795918"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3045,7 +3109,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -3281,10 +3345,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>21</v>
@@ -3304,10 +3368,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>17</v>
@@ -3327,10 +3391,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>21</v>
@@ -3350,10 +3414,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>21</v>
@@ -3392,22 +3456,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.5918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.61224489795918"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3415,7 +3479,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -3628,10 +3692,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>21</v>
@@ -3665,27 +3729,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y17"/>
+  <dimension ref="A1:Y20"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.9387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.6224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.61224489795918"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3693,7 +3757,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -3929,13 +3993,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>22</v>
@@ -3952,10 +4016,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>21</v>
@@ -3975,22 +4039,22 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H13" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I13" s="7" t="n">
         <v>1</v>
@@ -3998,13 +4062,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>22</v>
@@ -4021,22 +4085,22 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H15" s="7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I15" s="7" t="n">
         <v>1</v>
@@ -4044,13 +4108,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>22</v>
@@ -4067,24 +4131,93 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D18" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" s="7" t="n">
+      <c r="E18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4109,22 +4242,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.3571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.1836734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.61224489795918"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4132,7 +4265,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -4345,10 +4478,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
D8MT-1100: Update the mapping templates (EWCMS 1.21.2).
</commit_message>
<xml_diff>
--- a/templates/assets_mapping_template.xlsx
+++ b/templates/assets_mapping_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="D7 Inventory" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="111">
   <si>
     <t xml:space="preserve">Label</t>
   </si>
@@ -156,36 +156,30 @@
     <t xml:space="preserve">text</t>
   </si>
   <si>
-    <t xml:space="preserve">ewcms_description/format</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description / format</t>
+    <t xml:space="preserve">ewcms_file_thumbnail/target_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ewcms_file_thumbnail/alt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ewcms_file_thumbnail/title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ewcms_publication_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publication date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ewcms_resource_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource type</t>
   </si>
   <si>
     <t xml:space="preserve">varchar_ascii</t>
   </si>
   <si>
-    <t xml:space="preserve">ewcms_file_thumbnail/target_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ewcms_file_thumbnail/alt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ewcms_file_thumbnail/title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ewcms_publication_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Publication date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ewcms_resource_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource type</t>
-  </si>
-  <si>
     <t xml:space="preserve">ewcms_subject</t>
   </si>
   <si>
@@ -243,18 +237,21 @@
     <t xml:space="preserve">Remote File / title</t>
   </si>
   <si>
+    <t xml:space="preserve">oe_media_remote_file/options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remote File / options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blob</t>
+  </si>
+  <si>
     <t xml:space="preserve">oe_media_remote_file/size</t>
   </si>
   <si>
     <t xml:space="preserve">Remote File / size</t>
   </si>
   <si>
-    <t xml:space="preserve">oe_media_remote_file/format</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remote File / format</t>
-  </si>
-  <si>
     <t xml:space="preserve">iframe (iframe)</t>
   </si>
   <si>
@@ -343,18 +340,6 @@
   </si>
   <si>
     <t xml:space="preserve">Video iframe (video_iframe)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oe_media_iframe_thumbnail/width</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iframe thumbnail / width</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oe_media_iframe_thumbnail/height</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iframe thumbnail / height</t>
   </si>
   <si>
     <t xml:space="preserve">Webtools chart (webtools_chart)</t>
@@ -472,7 +457,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -499,10 +484,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -592,19 +573,19 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.25"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.95408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.0102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="8.1530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="25.1377551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -650,22 +631,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.25"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.6377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -673,7 +654,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -730,19 +711,19 @@
       <c r="D3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8" t="n">
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -753,19 +734,19 @@
       <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="8" t="n">
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -776,19 +757,19 @@
       <c r="D5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8" t="n">
+      <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -799,19 +780,19 @@
       <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8" t="n">
+      <c r="E6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -822,19 +803,19 @@
       <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8" t="n">
+      <c r="E7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -845,42 +826,42 @@
       <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8" t="n">
+      <c r="F8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="E9" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8" t="n">
+      <c r="F9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -905,22 +886,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="52.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="32"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="52.3775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -928,7 +909,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -985,19 +966,19 @@
       <c r="D3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8" t="n">
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1008,19 +989,19 @@
       <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="8" t="n">
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1031,19 +1012,19 @@
       <c r="D5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8" t="n">
+      <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1054,19 +1035,19 @@
       <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8" t="n">
+      <c r="E6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1077,19 +1058,19 @@
       <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8" t="n">
+      <c r="E7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1100,42 +1081,42 @@
       <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8" t="n">
+      <c r="F8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8" t="n">
+      <c r="F9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1157,25 +1138,25 @@
   </sheetPr>
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="39.7755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="39.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1183,7 +1164,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -1240,19 +1221,19 @@
       <c r="D3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8" t="n">
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1263,19 +1244,19 @@
       <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="8" t="n">
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1286,19 +1267,19 @@
       <c r="D5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8" t="n">
+      <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1309,19 +1290,19 @@
       <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8" t="n">
+      <c r="E6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1332,19 +1313,19 @@
       <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8" t="n">
+      <c r="E7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1355,42 +1336,42 @@
       <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8" t="n">
+      <c r="F8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E9" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8" t="n">
+      <c r="F9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1415,22 +1396,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1495,19 +1476,19 @@
       <c r="D3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="0" t="n">
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1518,19 +1499,19 @@
       <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="0" t="n">
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1541,19 +1522,19 @@
       <c r="D5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="0" t="n">
+      <c r="F5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1564,19 +1545,19 @@
       <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="0" t="n">
+      <c r="E6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1587,19 +1568,19 @@
       <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="0" t="n">
+      <c r="E7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1610,19 +1591,19 @@
       <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="0" t="n">
+      <c r="F8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1633,19 +1614,19 @@
       <c r="D9" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="0" t="n">
+      <c r="E9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1670,22 +1651,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1750,19 +1731,19 @@
       <c r="D3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="0" t="n">
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1773,19 +1754,19 @@
       <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="0" t="n">
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1796,19 +1777,19 @@
       <c r="D5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="0" t="n">
+      <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1819,19 +1800,19 @@
       <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="0" t="n">
+      <c r="E6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1842,19 +1823,19 @@
       <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="0" t="n">
+      <c r="E7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1865,19 +1846,19 @@
       <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="0" t="n">
+      <c r="F8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1888,19 +1869,19 @@
       <c r="D9" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="0" t="n">
+      <c r="E9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1920,27 +1901,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y26"/>
+  <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.8877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2005,19 +1986,19 @@
       <c r="D3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8" t="n">
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2028,19 +2009,19 @@
       <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="8" t="n">
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2051,19 +2032,19 @@
       <c r="D5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8" t="n">
+      <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2074,19 +2055,19 @@
       <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8" t="n">
+      <c r="E6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2097,19 +2078,19 @@
       <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8" t="n">
+      <c r="E7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2120,19 +2101,19 @@
       <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8" t="n">
+      <c r="F8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2143,19 +2124,19 @@
       <c r="D9" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8" t="n">
+      <c r="F9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2164,113 +2145,113 @@
         <v>40</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="8" t="n">
+        <v>24</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="8" t="n">
+        <v>26</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="8" t="n">
+        <v>28</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="8" t="n">
+        <v>44</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="E14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="8" t="n">
+      <c r="F14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2281,43 +2262,43 @@
       <c r="D15" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="8" t="n">
-        <v>1</v>
+      <c r="E15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2327,20 +2308,20 @@
       <c r="D17" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>52</v>
+      <c r="E17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2350,20 +2331,20 @@
       <c r="D18" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>52</v>
+      <c r="E18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" s="7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2373,19 +2354,19 @@
       <c r="D19" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="8" t="n">
+      <c r="F19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2396,19 +2377,19 @@
       <c r="D20" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="8" t="n">
+      <c r="E20" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2419,19 +2400,19 @@
       <c r="D21" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="8" t="n">
+      <c r="E21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2442,19 +2423,19 @@
       <c r="D22" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H22" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" s="8" t="n">
+      <c r="E22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2465,19 +2446,19 @@
       <c r="D23" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" s="8" t="n">
+      <c r="E23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2488,65 +2469,42 @@
       <c r="D24" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I24" s="8" t="n">
+      <c r="E24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I25" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H26" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" s="8" t="n">
+      <c r="F25" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2571,22 +2529,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.3520408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.9387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.6224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2594,7 +2552,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -2651,19 +2609,19 @@
       <c r="D3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8" t="n">
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2674,19 +2632,19 @@
       <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="8" t="n">
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2697,19 +2655,19 @@
       <c r="D5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8" t="n">
+      <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2720,19 +2678,19 @@
       <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8" t="n">
+      <c r="E6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2743,19 +2701,19 @@
       <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8" t="n">
+      <c r="E7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2766,157 +2724,157 @@
       <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8" t="n">
+      <c r="F8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8" t="n">
+      <c r="E9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="8" t="n">
+      <c r="F10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="8" t="n">
+      <c r="E11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="8" t="n">
+      <c r="F12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="8" t="n">
+      <c r="E13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="8" t="n">
+      <c r="E14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2941,22 +2899,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
+      <selection pane="bottomLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.9642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2964,7 +2922,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -3021,19 +2979,19 @@
       <c r="D3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8" t="n">
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3044,19 +3002,19 @@
       <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="8" t="n">
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3067,19 +3025,19 @@
       <c r="D5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8" t="n">
+      <c r="F5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3090,19 +3048,19 @@
       <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8" t="n">
+      <c r="E6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3113,19 +3071,19 @@
       <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8" t="n">
+      <c r="E7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3136,180 +3094,180 @@
       <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8" t="n">
+      <c r="F8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8" t="n">
+      <c r="E9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="8" t="n">
+      <c r="E10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="8" t="n">
+      <c r="F11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="8" t="n">
+      <c r="E12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="8" t="n">
+      <c r="E13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="8" t="n">
+      <c r="F14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="8" t="n">
+      <c r="F15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3334,22 +3292,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.5918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3357,7 +3315,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -3414,19 +3372,19 @@
       <c r="D3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8" t="n">
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3437,19 +3395,19 @@
       <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="8" t="n">
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3460,19 +3418,19 @@
       <c r="D5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8" t="n">
+      <c r="F5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3483,19 +3441,19 @@
       <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8" t="n">
+      <c r="E6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3506,19 +3464,19 @@
       <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8" t="n">
+      <c r="E7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3529,42 +3487,42 @@
       <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8" t="n">
+      <c r="F8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8" t="n">
+      <c r="E9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3584,27 +3542,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y18"/>
+  <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="bottomLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.219387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3612,7 +3570,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -3669,19 +3627,19 @@
       <c r="D3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="0" t="n">
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3692,19 +3650,19 @@
       <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="0" t="n">
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3715,19 +3673,19 @@
       <c r="D5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="0" t="n">
+      <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3738,19 +3696,19 @@
       <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="0" t="n">
+      <c r="E6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3761,19 +3719,19 @@
       <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="0" t="n">
+      <c r="E7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3784,19 +3742,19 @@
       <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="0" t="n">
+      <c r="F8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I8" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3807,226 +3765,180 @@
       <c r="D9" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="0" t="n">
+      <c r="F9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="0" t="n">
+      <c r="E10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="0" t="n">
+      <c r="E11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="0" t="n">
+      <c r="F12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="I12" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="0" t="n">
+      <c r="E13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="I13" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="0" t="n">
+      <c r="F14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="0" t="n">
+      <c r="E15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="0" t="n">
+      <c r="E16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4056,17 +3968,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.3571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.1836734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4074,7 +3986,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -4131,19 +4043,19 @@
       <c r="D3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8" t="n">
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4154,19 +4066,19 @@
       <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="8" t="n">
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4177,19 +4089,19 @@
       <c r="D5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8" t="n">
+      <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4200,19 +4112,19 @@
       <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8" t="n">
+      <c r="E6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4223,19 +4135,19 @@
       <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8" t="n">
+      <c r="E7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4246,42 +4158,42 @@
       <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8" t="n">
+      <c r="F8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="E9" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8" t="n">
+      <c r="F9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
D8MT-1100: Update the mapping templates (EWCMS 1.22.0).
</commit_message>
<xml_diff>
--- a/templates/assets_mapping_template.xlsx
+++ b/templates/assets_mapping_template.xlsx
@@ -573,19 +573,19 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.25"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.95408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.0102040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="8.1530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="25.1377551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="7.29081632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -631,22 +631,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.25"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.6377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -886,22 +886,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
+      <selection pane="bottomLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="52.3775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="52.9795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="32"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1141,22 +1141,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="39.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="39.7755102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1396,22 +1396,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.1632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.0510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1651,22 +1651,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1906,22 +1906,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.3061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.8877551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1996,7 +1996,7 @@
         <v>18</v>
       </c>
       <c r="H3" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="7" t="n">
         <v>1</v>
@@ -2019,7 +2019,7 @@
         <v>22</v>
       </c>
       <c r="H4" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="7" t="n">
         <v>1</v>
@@ -2042,7 +2042,7 @@
         <v>18</v>
       </c>
       <c r="H5" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="7" t="n">
         <v>1</v>
@@ -2065,7 +2065,7 @@
         <v>18</v>
       </c>
       <c r="H6" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="7" t="n">
         <v>1</v>
@@ -2111,7 +2111,7 @@
         <v>18</v>
       </c>
       <c r="H8" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="7" t="n">
         <v>1</v>
@@ -2226,7 +2226,7 @@
         <v>18</v>
       </c>
       <c r="H13" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="7" t="n">
         <v>1</v>
@@ -2249,7 +2249,7 @@
         <v>22</v>
       </c>
       <c r="H14" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="7" t="n">
         <v>1</v>
@@ -2341,7 +2341,7 @@
         <v>18</v>
       </c>
       <c r="H18" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="7" t="n">
         <v>1</v>
@@ -2410,7 +2410,7 @@
         <v>22</v>
       </c>
       <c r="H21" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" s="7" t="n">
         <v>1</v>
@@ -2529,22 +2529,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.4540816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.6224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.3520408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.9387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2899,22 +2899,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.0765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.9642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3292,22 +3292,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="K39" activeCellId="0" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.5918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3547,22 +3547,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="bottomLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.9387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3963,22 +3963,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.3571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.1836734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
D8MT-1100: Update the mapping templates (EWCMS 1.24.0).
</commit_message>
<xml_diff>
--- a/templates/assets_mapping_template.xlsx
+++ b/templates/assets_mapping_template.xlsx
@@ -5,24 +5,25 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="D7 Inventory" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="MAPPING - ... to AV Portal Photo (av_portal_photo)" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="MAPPING - ... to AV Portal Video (av_portal_video)" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="MAPPING - ... to Document (document)" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="MAPPING - ... to iframe (iframe)" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="MAPPING - ... to AV Portal Phot" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="MAPPING - ... to AV Portal Vide" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="MAPPING - ... to Document (docu" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="MAPPING - ... to iframe (iframe" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="MAPPING - ... to Image (image)" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="MAPPING - ... to Remote video (remote_video)" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="MAPPING - ... to Video iframe (video_iframe)" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="MAPPING - ... to Webtools chart (webtools_chart)" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="MAPPING - ... to Webtools map (webtools_map)" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="MAPPING - ... to Webtools op publication list (webtools_op_publication_list)" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="MAPPING - ... to Webtools social feed (webtools_social_feed)" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="MAPPING - ... to JavaScript ass" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="MAPPING - ... to Remote video (" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="MAPPING - ... to Video iframe (" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="MAPPING - ... to Webtools chart" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="MAPPING - ... to Webtools map (" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="MAPPING - ... to Webtools op pu" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="MAPPING - ... to Webtools socia" sheetId="13" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="tbl_dest" vbProcedure="false">'MAPPING - ... to AV Portal Photo (av_portal_photo)'!$C$2:$I$2</definedName>
+    <definedName function="false" hidden="false" name="tbl_dest" vbProcedure="false">'MAPPING - ... to AV Portal Phot'!$C$2:$I$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="113">
   <si>
     <t xml:space="preserve">Label</t>
   </si>
@@ -237,15 +238,6 @@
     <t xml:space="preserve">Remote File / title</t>
   </si>
   <si>
-    <t xml:space="preserve">oe_media_remote_file/options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remote File / options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blob</t>
-  </si>
-  <si>
     <t xml:space="preserve">oe_media_remote_file/size</t>
   </si>
   <si>
@@ -328,6 +320,21 @@
   </si>
   <si>
     <t xml:space="preserve">Image / height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JavaScript asset (javascript_asset)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_media_js_asset_url/environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JavaScript asset URL / environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_media_js_asset_url/path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JavaScript asset URL / path</t>
   </si>
   <si>
     <t xml:space="preserve">Remote video (remote_video)</t>
@@ -496,12 +503,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -567,25 +574,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="7.30078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="7.29081632653061"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="7.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="24.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.61"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="7.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -613,7 +620,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -622,31 +629,31 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.25"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.6377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -654,7 +661,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -844,7 +851,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>106</v>
@@ -868,7 +875,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -877,31 +884,31 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="bottomLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="52.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="32"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1099,7 +1106,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>108</v>
@@ -1123,7 +1130,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1132,31 +1139,31 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+      <selection pane="bottomLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="39.7755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="52.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1354,7 +1361,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>110</v>
@@ -1378,7 +1385,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1386,32 +1393,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.1632653061224"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.0510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="39.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="24.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1419,7 +1426,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>5</v>
+        <v>111</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -1526,7 +1533,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>18</v>
@@ -1549,7 +1556,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>18</v>
@@ -1572,7 +1579,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>18</v>
@@ -1609,13 +1616,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>32</v>
+        <v>112</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>18</v>
@@ -1633,7 +1640,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1641,32 +1648,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.6071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1674,7 +1681,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -1781,7 +1788,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>18</v>
@@ -1804,7 +1811,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>18</v>
@@ -1827,7 +1834,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>18</v>
@@ -1864,10 +1871,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>21</v>
@@ -1888,7 +1895,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1896,32 +1903,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="bottomLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.8877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1929,7 +1936,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -2119,399 +2126,31 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H21" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I24" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I25" s="7" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2519,32 +2158,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y14"/>
+  <dimension ref="A1:Y24"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.3520408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.9387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="30.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2552,7 +2191,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -2742,13 +2381,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>22</v>
@@ -2765,19 +2404,19 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H10" s="7" t="n">
         <v>0</v>
@@ -2788,16 +2427,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>18</v>
@@ -2811,16 +2450,16 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>18</v>
@@ -2834,16 +2473,16 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>18</v>
@@ -2857,31 +2496,261 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H14" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I14" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="7" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2889,32 +2758,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y15"/>
+  <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+      <selection pane="bottomLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.9642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2922,7 +2791,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -3029,7 +2898,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>18</v>
@@ -3052,7 +2921,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>18</v>
@@ -3075,7 +2944,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>18</v>
@@ -3112,10 +2981,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>21</v>
@@ -3135,19 +3004,19 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H10" s="7" t="n">
         <v>0</v>
@@ -3158,19 +3027,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H11" s="7" t="n">
         <v>0</v>
@@ -3181,19 +3050,19 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H12" s="7" t="n">
         <v>0</v>
@@ -3204,10 +3073,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>21</v>
@@ -3216,7 +3085,7 @@
         <v>22</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H13" s="7" t="n">
         <v>0</v>
@@ -3227,54 +3096,31 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H14" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I14" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="7" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3282,32 +3128,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K39" activeCellId="0" sqref="K39"/>
+      <selection pane="bottomLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3315,7 +3161,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -3505,10 +3351,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>21</v>
@@ -3517,19 +3363,157 @@
         <v>22</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="7" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3537,32 +3521,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y16"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+      <selection pane="bottomLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.9387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3570,7 +3554,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -3631,13 +3615,13 @@
         <v>17</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="H3" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I3" s="7" t="n">
         <v>1</v>
@@ -3660,7 +3644,7 @@
         <v>22</v>
       </c>
       <c r="H4" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I4" s="7" t="n">
         <v>1</v>
@@ -3677,13 +3661,13 @@
         <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>18</v>
       </c>
       <c r="H5" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I5" s="7" t="n">
         <v>1</v>
@@ -3700,13 +3684,13 @@
         <v>21</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>18</v>
       </c>
       <c r="H6" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I6" s="7" t="n">
         <v>1</v>
@@ -3723,7 +3707,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>18</v>
@@ -3746,13 +3730,13 @@
         <v>17</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>18</v>
       </c>
       <c r="H8" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I8" s="7" t="n">
         <v>1</v>
@@ -3760,19 +3744,19 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H9" s="7" t="n">
         <v>0</v>
@@ -3783,169 +3767,31 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H10" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I10" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="I12" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="I13" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" s="7" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3953,32 +3799,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+      <selection pane="bottomLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.3571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.1836734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="6.20918367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3986,7 +3832,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -4093,7 +3939,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>18</v>
@@ -4116,7 +3962,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>18</v>
@@ -4139,7 +3985,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>18</v>
@@ -4176,16 +4022,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>22</v>
@@ -4200,7 +4046,423 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Y16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
D8MT-1100: Update the mapping templates (EWCMS 1.26.1).
</commit_message>
<xml_diff>
--- a/templates/assets_mapping_template.xlsx
+++ b/templates/assets_mapping_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="D7 Inventory" sheetId="1" state="visible" r:id="rId2"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="124">
   <si>
     <t xml:space="preserve">Label</t>
   </si>
@@ -130,6 +130,12 @@
     <t xml:space="preserve">Authored on</t>
   </si>
   <si>
+    <t xml:space="preserve">ewcms_highlighted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Highlighted</t>
+  </si>
+  <si>
     <t xml:space="preserve">oe_media_avportal_photo</t>
   </si>
   <si>
@@ -238,12 +244,27 @@
     <t xml:space="preserve">Remote File / title</t>
   </si>
   <si>
+    <t xml:space="preserve">oe_media_remote_file/options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remote File / options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blob</t>
+  </si>
+  <si>
     <t xml:space="preserve">oe_media_remote_file/size</t>
   </si>
   <si>
     <t xml:space="preserve">Remote File / size</t>
   </si>
   <si>
+    <t xml:space="preserve">oe_media_remote_file/format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remote File / format</t>
+  </si>
+  <si>
     <t xml:space="preserve">iframe (iframe)</t>
   </si>
   <si>
@@ -281,6 +302,18 @@
   </si>
   <si>
     <t xml:space="preserve">Iframe thumbnail / title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_media_iframe_thumbnail/width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iframe thumbnail / width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_media_iframe_thumbnail/height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iframe thumbnail / height</t>
   </si>
   <si>
     <t xml:space="preserve">Image (image)</t>
@@ -580,7 +613,7 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -588,8 +621,8 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="7.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="24.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.61"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="7.29"/>
@@ -633,25 +666,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="G35" activeCellId="0" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.46"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
@@ -661,7 +694,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -851,24 +884,47 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>105</v>
+        <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>106</v>
+        <v>32</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -888,25 +944,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.46"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
@@ -916,7 +972,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -1106,24 +1162,47 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>105</v>
+        <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>108</v>
+        <v>32</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1143,25 +1222,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="52.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="52.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.46"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
@@ -1171,7 +1250,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -1361,24 +1440,47 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>105</v>
+        <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>110</v>
+        <v>32</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1398,25 +1500,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+      <selection pane="bottomLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="39.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="24.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="39.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.46"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
@@ -1426,7 +1528,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -1616,24 +1718,47 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>105</v>
+        <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1653,25 +1778,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.46"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
@@ -1877,18 +2002,41 @@
         <v>32</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1908,25 +2056,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+      <selection pane="bottomLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.46"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
@@ -1936,7 +2084,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -2126,24 +2274,47 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2163,25 +2334,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y24"/>
+  <dimension ref="A1:Y27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="30.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="30.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.46"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
@@ -2191,7 +2362,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -2381,13 +2552,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>22</v>
@@ -2404,16 +2575,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="E10" s="7" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>18</v>
@@ -2427,13 +2598,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>18</v>
@@ -2450,10 +2621,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>21</v>
@@ -2473,10 +2644,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>21</v>
@@ -2502,13 +2673,13 @@
         <v>46</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>18</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H14" s="7" t="n">
         <v>0</v>
@@ -2519,48 +2690,48 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="E15" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>47</v>
-      </c>
       <c r="F15" s="8" t="s">
         <v>18</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H15" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I15" s="7" t="s">
-        <v>50</v>
+      <c r="I15" s="7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="E16" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2571,7 +2742,7 @@
         <v>54</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>18</v>
@@ -2583,7 +2754,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2594,10 +2765,10 @@
         <v>56</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>18</v>
@@ -2605,8 +2776,8 @@
       <c r="H18" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I18" s="7" t="n">
-        <v>1</v>
+      <c r="I18" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2640,7 +2811,7 @@
         <v>60</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>22</v>
@@ -2663,13 +2834,13 @@
         <v>62</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H21" s="7" t="n">
         <v>0</v>
@@ -2692,7 +2863,7 @@
         <v>22</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H22" s="7" t="n">
         <v>0</v>
@@ -2732,7 +2903,7 @@
         <v>68</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>22</v>
@@ -2744,6 +2915,75 @@
         <v>0</v>
       </c>
       <c r="I24" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2763,25 +3003,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y14"/>
+  <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.46"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
@@ -2791,7 +3031,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -2981,13 +3221,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>22</v>
@@ -3004,19 +3244,19 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H10" s="7" t="n">
         <v>0</v>
@@ -3027,19 +3267,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H11" s="7" t="n">
         <v>0</v>
@@ -3050,13 +3290,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>22</v>
@@ -3073,13 +3313,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>22</v>
@@ -3096,10 +3336,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>21</v>
@@ -3114,6 +3354,75 @@
         <v>0</v>
       </c>
       <c r="I14" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3133,25 +3442,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y15"/>
+  <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.46"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
@@ -3161,7 +3470,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -3218,7 +3527,7 @@
       <c r="D3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -3241,7 +3550,7 @@
       <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="0" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="8" t="s">
@@ -3264,7 +3573,7 @@
       <c r="D5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
@@ -3287,7 +3596,7 @@
       <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="0" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="8" t="s">
@@ -3310,7 +3619,7 @@
       <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="0" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
@@ -3333,7 +3642,7 @@
       <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="8" t="s">
@@ -3351,13 +3660,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>22</v>
@@ -3374,12 +3683,12 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="8" t="s">
@@ -3397,19 +3706,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>17</v>
+        <v>95</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H11" s="7" t="n">
         <v>0</v>
@@ -3420,13 +3729,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>21</v>
+        <v>97</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>22</v>
@@ -3443,12 +3752,12 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="E13" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>21</v>
       </c>
       <c r="F13" s="8" t="s">
@@ -3466,13 +3775,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>17</v>
+        <v>101</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>22</v>
@@ -3489,12 +3798,12 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="E15" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="8" t="s">
@@ -3507,6 +3816,29 @@
         <v>0</v>
       </c>
       <c r="I15" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3526,25 +3858,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y10"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="30.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.46"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
@@ -3554,7 +3886,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -3744,19 +4076,19 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>96</v>
+        <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>97</v>
+        <v>32</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H9" s="7" t="n">
         <v>0</v>
@@ -3767,10 +4099,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>21</v>
@@ -3785,6 +4117,29 @@
         <v>0</v>
       </c>
       <c r="I10" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3804,25 +4159,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.46"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
@@ -3832,7 +4187,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -4022,24 +4377,47 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>101</v>
+        <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>102</v>
+        <v>32</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4059,25 +4437,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y16"/>
+  <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="15.46"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="10" style="1" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="6.21"/>
   </cols>
@@ -4087,7 +4465,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -4277,13 +4655,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>22</v>
@@ -4292,7 +4670,7 @@
         <v>18</v>
       </c>
       <c r="H9" s="7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I9" s="7" t="n">
         <v>1</v>
@@ -4300,13 +4678,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>22</v>
@@ -4323,10 +4701,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>21</v>
@@ -4346,22 +4724,22 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H12" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I12" s="7" t="n">
         <v>1</v>
@@ -4369,13 +4747,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>22</v>
@@ -4392,22 +4770,22 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H14" s="7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I14" s="7" t="n">
         <v>1</v>
@@ -4415,13 +4793,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>22</v>
@@ -4438,10 +4816,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>21</v>
@@ -4456,6 +4834,75 @@
         <v>0</v>
       </c>
       <c r="I16" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="7" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>